<commit_message>
excel sums to 1440 on every column
</commit_message>
<xml_diff>
--- a/datasets/Time_Use_in_OECD_Countries_OECD_after.xlsx
+++ b/datasets/Time_Use_in_OECD_Countries_OECD_after.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoantonio/Documents/Work2_EM/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449AA861-6EAA-3D45-BC6B-F49A229AAF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F30290-EA8E-0640-9B79-4E8069F6653D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20480" windowHeight="25100" xr2:uid="{AC39DB29-4830-4446-868B-914D3F2238E3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{AC39DB29-4830-4446-868B-914D3F2238E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Time Use (OECD)" sheetId="1" r:id="rId1"/>
@@ -248,7 +248,7 @@
     <definedName name="wrn.R22_Data_Collection1997." hidden="1">{"_R22_General",#N/A,TRUE,"R22_General";"_R22_Questions",#N/A,TRUE,"R22_Questions";"ColA_R22",#N/A,TRUE,"R2295";"_R22_Tables",#N/A,TRUE,"R2295"}</definedName>
     <definedName name="wrn.TabARA." hidden="1">{"Page1",#N/A,FALSE,"ARA M&amp;F&amp;T";"Page2",#N/A,FALSE,"ARA M&amp;F&amp;T";"Page3",#N/A,FALSE,"ARA M&amp;F&amp;T"}</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -804,7 +804,7 @@
   <dimension ref="A1:O34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L43" sqref="L43"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1472,7 +1472,8 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>325.7113724006864</v>
+        <f>325.711372400686-24</f>
+        <v>301.711372400686</v>
       </c>
       <c r="C15" s="1">
         <v>36.979999999999997</v>
@@ -1502,7 +1503,7 @@
         <v>10.222599959407347</v>
       </c>
       <c r="L15" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M15" s="1">
         <v>16.912066166023951</v>
@@ -1707,7 +1708,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>302.33356400000002</v>
+        <v>304.33356400000002</v>
       </c>
       <c r="C20" s="1">
         <v>45.29898</v>
@@ -1801,7 +1802,8 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>240.99999999999997</v>
+        <f>241-2</f>
+        <v>239</v>
       </c>
       <c r="C22" s="1">
         <v>29</v>
@@ -2083,7 +2085,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>262.18713699086243</v>
+        <v>268.18713699086197</v>
       </c>
       <c r="C28" s="1">
         <v>31.219734784113403</v>
@@ -2130,7 +2132,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>217.02784000000003</v>
+        <v>217.02784</v>
       </c>
       <c r="C29" s="1">
         <v>29.041440000000001</v>
@@ -2177,7 +2179,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>235.49323385367586</v>
+        <v>234.493233853676</v>
       </c>
       <c r="C30" s="1">
         <v>26.771676014251472</v>
@@ -2365,7 +2367,8 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>188.80248</v>
+        <f>188.80248+13</f>
+        <v>201.80248</v>
       </c>
       <c r="C34" s="1">
         <v>38.810659999999999</v>
@@ -2410,7 +2413,7 @@
   </sheetData>
   <autoFilter ref="A1:B34" xr:uid="{8A7DEDFF-A262-B743-9D57-742C85F41536}"/>
   <conditionalFormatting sqref="C1">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2422,7 +2425,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2434,7 +2437,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="dataBar" priority="19">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2446,7 +2449,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2458,7 +2461,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2470,7 +2473,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2482,7 +2485,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="dataBar" priority="15">
+    <cfRule type="dataBar" priority="16">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2494,7 +2497,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2506,7 +2509,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2518,7 +2521,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2530,7 +2533,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1">
-    <cfRule type="dataBar" priority="11">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2542,7 +2545,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2554,7 +2557,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2566,7 +2569,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2578,7 +2581,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2590,7 +2593,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2602,7 +2605,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2614,7 +2617,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2626,7 +2629,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2638,7 +2641,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2650,7 +2653,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2662,7 +2665,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2674,7 +2677,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O1">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="26">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2686,7 +2689,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>